<commit_message>
update version ci-build 96ec884b285207e453456cb6acee30ea5e555f43
</commit_message>
<xml_diff>
--- a/sd-040-ballot1-cibuild/ig/CodeSystem-act-type-ror-codesystem.xlsx
+++ b/sd-040-ballot1-cibuild/ig/CodeSystem-act-type-ror-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.3.0</t>
+    <t>0.4.0-ballot-1</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-13T15:02:17+00:00</t>
+    <t>2024-03-13T16:17:04+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>